<commit_message>
working team stats frontend
</commit_message>
<xml_diff>
--- a/stat_explanations.xlsx
+++ b/stat_explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="231">
   <si>
     <t>team stats</t>
   </si>
@@ -785,8 +785,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -897,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -948,6 +950,7 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -998,6 +1001,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1327,11 +1331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O144"/>
+  <dimension ref="A1:P144"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G105" sqref="G105:G144"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1340,15 +1344,15 @@
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="58.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" customWidth="1"/>
     <col min="9" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="14" width="24.5" customWidth="1"/>
-    <col min="15" max="15" width="15.5" customWidth="1"/>
+    <col min="10" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="15" width="24.5" customWidth="1"/>
+    <col min="16" max="16" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1380,31 +1384,31 @@
         <v>230</v>
       </c>
       <c r="K1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" t="s">
         <v>186</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>188</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>122</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>123</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>124</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1415,16 +1419,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>168</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1435,16 +1436,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>182</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1452,16 +1450,13 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>181</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1472,16 +1467,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>125</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1495,16 +1487,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>167</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1518,16 +1507,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>126</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1535,16 +1521,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>117</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1554,21 +1537,18 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1578,12 +1558,12 @@
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1594,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1631,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1648,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1664,12 +1644,12 @@
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1685,12 +1665,12 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1724,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1738,7 +1718,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1752,7 +1732,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1766,7 +1746,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1783,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1800,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1817,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1834,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1848,7 +1828,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1865,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1873,7 +1853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1889,12 +1869,12 @@
       <c r="I29">
         <v>1</v>
       </c>
-      <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1911,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1925,7 +1905,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="A32" s="6" t="s">
         <v>106</v>
       </c>
@@ -1939,7 +1919,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" s="6" t="s">
         <v>107</v>
       </c>
@@ -1953,7 +1933,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1967,7 +1947,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1981,7 +1961,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1992,7 +1972,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2003,7 +1983,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2020,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2034,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2048,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2065,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2079,7 +2059,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2095,12 +2075,12 @@
       <c r="I43">
         <v>1</v>
       </c>
-      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2117,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2134,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2148,7 +2128,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2164,12 +2144,12 @@
       <c r="I47">
         <v>1</v>
       </c>
-      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2469,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2480,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2488,7 +2468,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2499,7 +2479,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2513,7 +2493,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -2530,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2547,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2558,7 +2538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2575,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2592,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2608,12 +2588,12 @@
       <c r="I90">
         <v>1</v>
       </c>
-      <c r="K90" s="1"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="O90" s="1"/>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2630,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -2647,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2663,12 +2643,12 @@
       <c r="I93">
         <v>1</v>
       </c>
-      <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="O93" s="1"/>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -2682,7 +2662,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2699,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
new bower components, stats crawling functions
</commit_message>
<xml_diff>
--- a/stat_explanations.xlsx
+++ b/stat_explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="232">
   <si>
     <t>team stats</t>
   </si>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>similarity vector</t>
+  </si>
+  <si>
+    <t>Personal fouls drawn</t>
   </si>
 </sst>
 </file>
@@ -1333,9 +1336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P144"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H122" sqref="H122"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2456,6 +2459,9 @@
       <c r="G81" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="H81" t="s">
+        <v>231</v>
+      </c>
       <c r="I81">
         <v>1</v>
       </c>
@@ -2463,6 +2469,9 @@
     <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>231</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>82</v>

</xml_diff>